<commit_message>
Plugin Temperatur, Static, Navi - Ready
Diese Plugins sind fertig, müssen aber noch überarbeitet werden
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Zeitliste" sheetId="1" r:id="rId1"/>
     <sheet name="Zeitliste Pivot" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
     <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>Interfaces verstehen und erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plugin Static - Probleme bei der Bildübertragung - Flush </t>
+  </si>
+  <si>
+    <t>Plugin Navi - Multiuserfähigkeit</t>
+  </si>
+  <si>
+    <t>Plugin Static, Plugin Navi</t>
+  </si>
+  <si>
+    <t>Plugin Navi</t>
   </si>
 </sst>
 </file>
@@ -268,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -343,6 +355,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -729,11 +744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-505504240"/>
-        <c:axId val="-505502608"/>
+        <c:axId val="540843616"/>
+        <c:axId val="540846880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-505504240"/>
+        <c:axId val="540843616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,7 +772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-505502608"/>
+        <c:crossAx val="540846880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -765,7 +780,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-505502608"/>
+        <c:axId val="540846880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,7 +806,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-505504240"/>
+        <c:crossAx val="540843616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -844,13 +859,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41553.528099768519" refreshedVersion="5" recordCount="148">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41603.316603472224" refreshedVersion="5" recordCount="148">
   <cacheSource type="worksheet">
     <worksheetSource ref="A4:E152" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-10-06T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-10-07T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -940,11 +955,11 @@
     <s v="Plugin Temperatur"/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="3"/>
-    <m/>
-    <m/>
+    <d v="2013-10-06T00:00:00"/>
+    <x v="1"/>
+    <x v="2"/>
+    <m/>
+    <s v="Interfaces verstehen und erstellen"/>
   </r>
   <r>
     <m/>
@@ -1999,9 +2014,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2039,7 +2054,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2111,7 +2126,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2264,7 +2279,7 @@
   <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2462,32 +2477,72 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="23">
+        <v>41600</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="23">
+        <v>41601</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="23">
+        <v>41602</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="23">
+        <v>41603</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>

</xml_diff>

<commit_message>
Plugin 4 - RssFeed
Fehlt noch:
Funktioniert
Try-Catch
ParseParameter
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitliste" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="55">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Summe von Dauer (h)</t>
+  </si>
+  <si>
+    <t>Error-Handling</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -739,7 +741,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -877,18 +879,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-72040656"/>
-        <c:axId val="-72043920"/>
+        <c:axId val="440202592"/>
+        <c:axId val="440193344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-72040656"/>
+        <c:axId val="440202592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -902,10 +903,10 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-72043920"/>
+        <c:crossAx val="440193344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -913,7 +914,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-72043920"/>
+        <c:axId val="440193344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,17 +937,16 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-72040656"/>
+        <c:crossAx val="440202592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -992,13 +992,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41611.502424768521" refreshedVersion="5" recordCount="164">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41623.895816203702" refreshedVersion="5" recordCount="164">
   <cacheSource type="worksheet">
     <worksheetSource ref="A4:E168" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-12-04T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-12-16T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1358,11 +1358,11 @@
     <m/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="7"/>
-    <m/>
-    <m/>
+    <d v="2013-12-15T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2"/>
+    <s v="Error-Handling"/>
   </r>
   <r>
     <m/>
@@ -2279,9 +2279,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2319,7 +2319,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2391,7 +2391,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2543,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3332,82 +3332,94 @@
       <c r="C48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="23">
+        <v>41623</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="3">
+        <v>4</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="E64" s="1"/>
@@ -3964,7 +3976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D12"/>
       <pivotSelection pane="bottomRight" showHeader="1" activeRow="2" click="1" r:id="rId1">
         <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
@@ -4015,10 +4027,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="13">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="14">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4111,10 +4123,10 @@
         <v>35</v>
       </c>
       <c r="C12" s="21">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" s="22">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GetTemperatur = Temperatur + UnitTests
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="57">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Plugin 4 - RssFeed</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
   </si>
 </sst>
 </file>
@@ -744,7 +747,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -882,11 +885,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-184977392"/>
-        <c:axId val="-184976848"/>
+        <c:axId val="-1115648544"/>
+        <c:axId val="-1115645280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-184977392"/>
+        <c:axId val="-1115648544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +912,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-184976848"/>
+        <c:crossAx val="-1115645280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -917,7 +920,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-184976848"/>
+        <c:axId val="-1115645280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +946,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-184977392"/>
+        <c:crossAx val="-1115648544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -995,13 +998,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41631.759327546293" refreshedVersion="5" recordCount="164">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41633.846448958335" refreshedVersion="5" recordCount="164">
   <cacheSource type="worksheet">
     <worksheetSource ref="A4:E168" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-12-16T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-12-24T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1368,11 +1371,11 @@
     <s v="Error-Handling"/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="7"/>
-    <m/>
-    <m/>
+    <d v="2013-12-23T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="5"/>
+    <s v="Plugin 4 - RssFeed"/>
   </r>
   <r>
     <m/>
@@ -2547,7 +2550,7 @@
   <dimension ref="A1:E172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3375,9 +3378,21 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="A52" s="23">
+        <v>41633</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
@@ -4042,10 +4057,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="13">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D5" s="14">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4138,10 +4153,10 @@
         <v>35</v>
       </c>
       <c r="C12" s="21">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D12" s="22">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maybe LAST COMMIT =)
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Unit Tests Nr. 23</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,11 +888,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1115648544"/>
-        <c:axId val="-1115645280"/>
+        <c:axId val="-1629999824"/>
+        <c:axId val="-1629993296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1115648544"/>
+        <c:axId val="-1629999824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,7 +915,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1115645280"/>
+        <c:crossAx val="-1629993296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -920,7 +923,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1115645280"/>
+        <c:axId val="-1629993296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +949,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1115648544"/>
+        <c:crossAx val="-1629999824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,13 +1001,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41633.846448958335" refreshedVersion="5" recordCount="164">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Daniel Hö" refreshedDate="41635.848448032404" refreshedVersion="5" recordCount="164">
   <cacheSource type="worksheet">
     <worksheetSource ref="A4:E168" sheet="Zeitliste"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Datum" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-12-24T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-09-26T00:00:00" maxDate="2013-12-26T00:00:00"/>
     </cacheField>
     <cacheField name="Ausführende/r" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1378,11 +1381,11 @@
     <s v="Plugin 4 - RssFeed"/>
   </r>
   <r>
-    <m/>
-    <x v="2"/>
-    <x v="7"/>
-    <m/>
-    <m/>
+    <d v="2013-12-25T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2"/>
+    <s v="Dokumentation"/>
   </r>
   <r>
     <m/>
@@ -2550,7 +2553,7 @@
   <dimension ref="A1:E172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3395,11 +3398,24 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="A53" s="23">
+        <v>41634</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="23"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="E54" s="1"/>
@@ -4057,10 +4073,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="13">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" s="14">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4153,10 +4169,10 @@
         <v>35</v>
       </c>
       <c r="C12" s="21">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="22">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>